<commit_message>
System Design, Design Patterns, and DSA update
10th March update in System Design, Design Patterns, and Programming DSA
</commit_message>
<xml_diff>
--- a/Programming/Revision_of_Blind_75_Questions_Shashank_1663097124.xlsx
+++ b/Programming/Revision_of_Blind_75_Questions_Shashank_1663097124.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreejitverma/Documents/GitHub/SDE Interview Prep/Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47688B8A-1B00-B74D-A02D-0700D006D4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E034F2E-C71F-6843-BE8B-D6CA66F69EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -959,7 +959,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -1081,6 +1081,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="1"/>
     </font>
@@ -1321,7 +1327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1385,6 +1391,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1749,7 +1758,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1801,7 +1810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1824,8 +1833,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1847,8 +1856,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1870,8 +1879,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1893,8 +1902,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1916,8 +1925,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1939,7 +1948,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1962,8 +1971,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1985,7 +1994,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -2008,8 +2017,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -2031,8 +2040,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -2054,14 +2063,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="21" t="s">
         <v>54</v>
       </c>
       <c r="D16" s="6">
@@ -2077,7 +2086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -2100,8 +2109,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>60</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -2123,8 +2132,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
         <v>63</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -2146,7 +2155,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>67</v>
       </c>
@@ -2169,8 +2178,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -2192,8 +2201,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
         <v>76</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -2215,8 +2224,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
         <v>80</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -2238,8 +2247,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
         <v>84</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -2261,8 +2270,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -2284,8 +2293,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
         <v>92</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -2307,8 +2316,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
         <v>96</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -2330,8 +2339,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
         <v>100</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -2353,7 +2362,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>104</v>
       </c>
@@ -2514,7 +2523,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>133</v>
       </c>
@@ -2537,8 +2546,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="22" t="s">
         <v>137</v>
       </c>
       <c r="B37" s="15" t="s">
@@ -2560,8 +2569,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="22" t="s">
         <v>142</v>
       </c>
       <c r="B38" s="15" t="s">
@@ -2583,7 +2592,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>146</v>
       </c>
@@ -3208,9 +3217,10 @@
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" xr:uid="{7B7015A9-A5F0-AF42-9EB1-7DB686C8464C}"/>
     <hyperlink ref="C12" r:id="rId2" xr:uid="{17F3CDCA-7DE6-9441-960B-1C975235C050}"/>
+    <hyperlink ref="C16" r:id="rId3" xr:uid="{EFCC80F8-ED7B-0449-A5D3-2D59EF837227}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>